<commit_message>
Updated Neural Network A1 - Analysis
</commit_message>
<xml_diff>
--- a/4-Analysis/Neural Network/Neural Network A1-test.xlsx
+++ b/4-Analysis/Neural Network/Neural Network A1-test.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\snegan\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\snegan\Documents\GitHub\AI-Build-Carbon-Predictor\4-Analysis\Neural Network\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{440F918E-3616-46C1-86E9-741EF554B4BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEE20E36-C739-47A8-AD65-B95849BD184D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Neural Network A1" sheetId="1" r:id="rId1"/>
@@ -764,9 +764,6 @@
   </cellStyles>
   <dxfs count="127">
     <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -775,6 +772,9 @@
     </dxf>
     <dxf>
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -1401,7 +1401,7 @@
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
+  <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>80963</xdr:colOff>
@@ -1411,147 +1411,137 @@
     <xdr:to>
       <xdr:col>2</xdr:col>
       <xdr:colOff>509588</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>523875</xdr:rowOff>
     </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Graphic 2" descr="Link">
-          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="2" name="Group 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{33B5F07E-1FDB-432B-6779-F456DB041590}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
-          <a:extLst>
-            <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
-              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId3"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
         <a:xfrm>
           <a:off x="2776538" y="3429000"/>
-          <a:ext cx="428625" cy="428625"/>
+          <a:ext cx="428625" cy="1219200"/>
+          <a:chOff x="2776538" y="3429000"/>
+          <a:chExt cx="428625" cy="1219200"/>
         </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>80963</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>14288</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>509588</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>23813</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Graphic 3" descr="Link">
-          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
-          <a:extLst>
-            <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
-              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId3"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="2776538" y="3929063"/>
-          <a:ext cx="428625" cy="428625"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>80963</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>509588</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>523875</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="5" name="Graphic 4" descr="Link">
-          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
-          <a:extLst>
-            <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
-              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId3"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="2776538" y="4429125"/>
-          <a:ext cx="428625" cy="428625"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
+      </xdr:grpSpPr>
+      <xdr:pic>
+        <xdr:nvPicPr>
+          <xdr:cNvPr id="3" name="Graphic 2" descr="Link">
+            <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvPicPr>
+            <a:picLocks noChangeAspect="1"/>
+          </xdr:cNvPicPr>
+        </xdr:nvPicPr>
+        <xdr:blipFill>
+          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+            <a:extLst>
+              <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
+                <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId3"/>
+              </a:ext>
+            </a:extLst>
+          </a:blip>
+          <a:stretch>
+            <a:fillRect/>
+          </a:stretch>
+        </xdr:blipFill>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="2776538" y="3429000"/>
+            <a:ext cx="428625" cy="428625"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+        </xdr:spPr>
+      </xdr:pic>
+      <xdr:pic>
+        <xdr:nvPicPr>
+          <xdr:cNvPr id="4" name="Graphic 3" descr="Link">
+            <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004000000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvPicPr>
+            <a:picLocks noChangeAspect="1"/>
+          </xdr:cNvPicPr>
+        </xdr:nvPicPr>
+        <xdr:blipFill>
+          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+            <a:extLst>
+              <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
+                <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId3"/>
+              </a:ext>
+            </a:extLst>
+          </a:blip>
+          <a:stretch>
+            <a:fillRect/>
+          </a:stretch>
+        </xdr:blipFill>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="2776538" y="3719513"/>
+            <a:ext cx="428625" cy="428625"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+        </xdr:spPr>
+      </xdr:pic>
+      <xdr:pic>
+        <xdr:nvPicPr>
+          <xdr:cNvPr id="5" name="Graphic 4" descr="Link">
+            <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005000000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvPicPr>
+            <a:picLocks noChangeAspect="1"/>
+          </xdr:cNvPicPr>
+        </xdr:nvPicPr>
+        <xdr:blipFill>
+          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+            <a:extLst>
+              <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
+                <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId3"/>
+              </a:ext>
+            </a:extLst>
+          </a:blip>
+          <a:stretch>
+            <a:fillRect/>
+          </a:stretch>
+        </xdr:blipFill>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="2776538" y="4219575"/>
+            <a:ext cx="428625" cy="428625"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+        </xdr:spPr>
+      </xdr:pic>
+    </xdr:grpSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -4041,7 +4031,7 @@
         <xdr:cNvPr id="2" name="Straight Arrow Connector 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{21689835-C01E-4EEF-927D-418AB350B1BC}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4094,7 +4084,7 @@
         <xdr:cNvPr id="3" name="Straight Arrow Connector 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C04B907E-FBD1-4090-BC6D-5E4F0C1D779F}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4147,7 +4137,7 @@
         <xdr:cNvPr id="4" name="Straight Arrow Connector 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8703EBF1-ECB2-4F1D-8806-1BC23B759985}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4200,7 +4190,7 @@
         <xdr:cNvPr id="5" name="Straight Arrow Connector 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D42B11D3-BBBC-4BC8-B535-85EFF4D2AE93}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4253,7 +4243,7 @@
         <xdr:cNvPr id="6" name="Straight Arrow Connector 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4C862FF4-41B8-4B43-BA79-8C759A23BC27}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000006000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4306,7 +4296,7 @@
         <xdr:cNvPr id="7" name="Straight Arrow Connector 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F259C3AA-3909-48C4-A18E-09C9F9744930}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000007000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4359,7 +4349,7 @@
         <xdr:cNvPr id="11" name="Straight Arrow Connector 10">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A38DECD5-E07E-4839-BCF0-00BA9ACB0A3B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-00000B000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4412,7 +4402,7 @@
         <xdr:cNvPr id="12" name="Straight Arrow Connector 11">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C130D1FE-892F-4956-BE80-3802F4474259}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-00000C000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4465,7 +4455,7 @@
         <xdr:cNvPr id="13" name="Straight Arrow Connector 12">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E88B8127-4C54-42BF-8019-DEA72B899E08}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-00000D000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4518,7 +4508,7 @@
         <xdr:cNvPr id="14" name="Straight Arrow Connector 13">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B5022C2B-5AC5-4DEC-A8C5-263210995963}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-00000E000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4557,23 +4547,23 @@
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
       <xdr:twoCellAnchor>
         <xdr:from>
-          <xdr:col>20</xdr:col>
+          <xdr:col>15</xdr:col>
           <xdr:colOff>114299</xdr:colOff>
-          <xdr:row>1</xdr:row>
-          <xdr:rowOff>95250</xdr:rowOff>
+          <xdr:row>2</xdr:row>
+          <xdr:rowOff>19050</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>22</xdr:col>
+          <xdr:col>17</xdr:col>
           <xdr:colOff>355890</xdr:colOff>
-          <xdr:row>11</xdr:row>
-          <xdr:rowOff>57150</xdr:rowOff>
+          <xdr:row>12</xdr:row>
+          <xdr:rowOff>47625</xdr:rowOff>
         </xdr:to>
         <xdr:grpSp>
           <xdr:nvGrpSpPr>
             <xdr:cNvPr id="15" name="Group 14">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ACE37601-95CE-4FEB-8843-5A7AF0099961}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-00000F000000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -4581,7 +4571,7 @@
           </xdr:nvGrpSpPr>
           <xdr:grpSpPr>
             <a:xfrm>
-              <a:off x="16306799" y="285750"/>
+              <a:off x="13258799" y="466725"/>
               <a:ext cx="1460791" cy="2019300"/>
               <a:chOff x="5105399" y="504825"/>
               <a:chExt cx="1457327" cy="1143000"/>
@@ -4595,7 +4585,7 @@
                     <a14:compatExt spid="_x0000_s6145"/>
                   </a:ext>
                   <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                    <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000001140000}"/>
+                    <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000001180000}"/>
                   </a:ext>
                 </a:extLst>
               </xdr:cNvPr>
@@ -4644,7 +4634,7 @@
                     <a14:compatExt spid="_x0000_s6146"/>
                   </a:ext>
                   <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                    <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000002140000}"/>
+                    <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000002180000}"/>
                   </a:ext>
                 </a:extLst>
               </xdr:cNvPr>
@@ -4693,7 +4683,7 @@
                     <a14:compatExt spid="_x0000_s6147"/>
                   </a:ext>
                   <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                    <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000003140000}"/>
+                    <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000003180000}"/>
                   </a:ext>
                 </a:extLst>
               </xdr:cNvPr>
@@ -5703,10 +5693,10 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="102" xr:uid="{1FD83134-0601-4AC9-AD53-860C252411BF}" name="Table469914137217678103" displayName="Table469914137217678103" ref="L11:O16" totalsRowShown="0">
   <autoFilter ref="L11:O16" xr:uid="{1FD83134-0601-4AC9-AD53-860C252411BF}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{D7ED44A4-6505-4548-A53B-9139E13BFB86}" name="Regularization" dataDxfId="0"/>
-    <tableColumn id="2" xr3:uid="{947DDC8F-6A59-4E1A-A388-E796ED6CEC79}" name="Accuracy (%)" dataDxfId="3"/>
-    <tableColumn id="3" xr3:uid="{4848E4B5-FA9D-45D2-8BF4-422F1B3B296A}" name="Time taken (t) / s" dataDxfId="2"/>
-    <tableColumn id="5" xr3:uid="{4F08D1FB-6F5C-4A08-A38A-0B2014395883}" name="Performance (1/t)" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{D7ED44A4-6505-4548-A53B-9139E13BFB86}" name="Regularization" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{947DDC8F-6A59-4E1A-A388-E796ED6CEC79}" name="Accuracy (%)" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{4848E4B5-FA9D-45D2-8BF4-422F1B3B296A}" name="Time taken (t) / s" dataDxfId="1"/>
+    <tableColumn id="5" xr3:uid="{4F08D1FB-6F5C-4A08-A38A-0B2014395883}" name="Performance (1/t)" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5978,8 +5968,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="B2:B25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M19" sqref="M19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F2" sqref="B2:F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6110,8 +6100,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="B2:J32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J35" sqref="J35"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L17" sqref="L17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6501,14 +6491,15 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x14">
       <controls>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="2049" r:id="rId3" name="Button 1">
+            <control shapeId="2049" r:id="rId4" name="Button 1">
               <controlPr defaultSize="0" print="0" autoFill="0" autoPict="0" macro="[0]!CalculateAverage">
                 <anchor moveWithCells="1" sizeWithCells="1">
                   <from>
@@ -6530,7 +6521,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="2050" r:id="rId4" name="Button 2">
+            <control shapeId="2050" r:id="rId5" name="Button 2">
               <controlPr defaultSize="0" print="0" autoFill="0" autoPict="0" macro="[0]!ProcessData">
                 <anchor moveWithCells="1" sizeWithCells="1">
                   <from>
@@ -6552,7 +6543,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="2051" r:id="rId5" name="Button 3">
+            <control shapeId="2051" r:id="rId6" name="Button 3">
               <controlPr defaultSize="0" print="0" autoFill="0" autoPict="0" macro="[0]!CalculateReciprocals">
                 <anchor moveWithCells="1" sizeWithCells="1">
                   <from>
@@ -6576,7 +6567,6 @@
     </mc:Choice>
   </mc:AlternateContent>
   <tableParts count="9">
-    <tablePart r:id="rId6"/>
     <tablePart r:id="rId7"/>
     <tablePart r:id="rId8"/>
     <tablePart r:id="rId9"/>
@@ -6585,6 +6575,7 @@
     <tablePart r:id="rId12"/>
     <tablePart r:id="rId13"/>
     <tablePart r:id="rId14"/>
+    <tablePart r:id="rId15"/>
   </tableParts>
 </worksheet>
 </file>
@@ -9104,7 +9095,7 @@
   <dimension ref="B2:O40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L28" sqref="L28"/>
+      <selection activeCell="S25" sqref="S25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9950,16 +9941,16 @@
               <controlPr defaultSize="0" print="0" autoFill="0" autoPict="0" macro="[0]!CalculateAverage">
                 <anchor moveWithCells="1">
                   <from>
-                    <xdr:col>20</xdr:col>
+                    <xdr:col>15</xdr:col>
                     <xdr:colOff>114300</xdr:colOff>
-                    <xdr:row>1</xdr:row>
-                    <xdr:rowOff>95250</xdr:rowOff>
+                    <xdr:row>2</xdr:row>
+                    <xdr:rowOff>19050</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>22</xdr:col>
+                    <xdr:col>17</xdr:col>
                     <xdr:colOff>352425</xdr:colOff>
-                    <xdr:row>3</xdr:row>
-                    <xdr:rowOff>180975</xdr:rowOff>
+                    <xdr:row>4</xdr:row>
+                    <xdr:rowOff>171450</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -9972,16 +9963,16 @@
               <controlPr defaultSize="0" print="0" autoFill="0" autoPict="0" macro="[0]!ProcessData">
                 <anchor moveWithCells="1" sizeWithCells="1">
                   <from>
-                    <xdr:col>20</xdr:col>
+                    <xdr:col>15</xdr:col>
                     <xdr:colOff>114300</xdr:colOff>
-                    <xdr:row>4</xdr:row>
-                    <xdr:rowOff>200025</xdr:rowOff>
+                    <xdr:row>5</xdr:row>
+                    <xdr:rowOff>180975</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>22</xdr:col>
+                    <xdr:col>17</xdr:col>
                     <xdr:colOff>352425</xdr:colOff>
-                    <xdr:row>7</xdr:row>
-                    <xdr:rowOff>142875</xdr:rowOff>
+                    <xdr:row>8</xdr:row>
+                    <xdr:rowOff>133350</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -9994,16 +9985,16 @@
               <controlPr defaultSize="0" print="0" autoFill="0" autoPict="0" macro="[0]!CalculateReciprocals">
                 <anchor moveWithCells="1" sizeWithCells="1">
                   <from>
-                    <xdr:col>20</xdr:col>
+                    <xdr:col>15</xdr:col>
                     <xdr:colOff>114300</xdr:colOff>
-                    <xdr:row>8</xdr:row>
-                    <xdr:rowOff>152400</xdr:rowOff>
+                    <xdr:row>9</xdr:row>
+                    <xdr:rowOff>142875</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>22</xdr:col>
+                    <xdr:col>17</xdr:col>
                     <xdr:colOff>352425</xdr:colOff>
-                    <xdr:row>11</xdr:row>
-                    <xdr:rowOff>57150</xdr:rowOff>
+                    <xdr:row>12</xdr:row>
+                    <xdr:rowOff>47625</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>

</xml_diff>